<commit_message>
adjusted data cleaning to new information
</commit_message>
<xml_diff>
--- a/Meat_Data.xlsx
+++ b/Meat_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon Kim\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon Kim\OneDrive\Desktop\School Stuff\Steak_Cutting_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460C84BA-D818-4C99-B438-94AF5C5A869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA43890-8395-428C-8438-64DACDE8B48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5220" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="everything one sheet" sheetId="47" r:id="rId1"/>
@@ -19324,7 +19324,7 @@
   <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19426,22 +19426,22 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="13">
-        <v>48.349999999999994</v>
+        <v>54.879999999999995</v>
       </c>
       <c r="F4" s="13">
-        <v>14.625</v>
+        <v>18.634999999999998</v>
       </c>
       <c r="G4" s="13">
-        <v>8.01</v>
+        <v>9.6449999999999996</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
@@ -19455,22 +19455,22 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" s="13">
-        <v>50.08</v>
+        <v>54.86</v>
       </c>
       <c r="F5" s="13">
-        <v>17.325000000000003</v>
+        <v>18.66</v>
       </c>
       <c r="G5" s="13">
-        <v>9.0599999999999987</v>
+        <v>9.27</v>
       </c>
       <c r="H5" t="s">
         <v>2</v>
@@ -19487,25 +19487,25 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" s="13">
-        <v>46.234999999999999</v>
+        <v>59.03</v>
       </c>
       <c r="F6" s="13">
-        <v>12.31</v>
+        <v>15.17</v>
       </c>
       <c r="G6" s="13">
-        <v>7.665</v>
+        <v>8.31</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -19516,25 +19516,25 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" s="13">
-        <v>48.094999999999999</v>
+        <v>52.96</v>
       </c>
       <c r="F7" s="13">
-        <v>14.91</v>
+        <v>15.24</v>
       </c>
       <c r="G7" s="13">
-        <v>8.66</v>
+        <v>7.02</v>
       </c>
       <c r="H7" t="s">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -19542,28 +19542,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="13">
-        <v>48.85</v>
+        <v>52.41</v>
       </c>
       <c r="F8" s="13">
-        <v>10.733333333333334</v>
+        <v>15.7</v>
       </c>
       <c r="G8" s="13">
-        <v>8.2266666666666666</v>
+        <v>7.71</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -19571,51 +19571,51 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" s="13">
-        <v>48</v>
+        <v>54.08</v>
       </c>
       <c r="F9" s="13">
-        <v>12.526666666666666</v>
+        <v>16.579999999999998</v>
       </c>
       <c r="G9" s="13">
-        <v>6.7600000000000007</v>
+        <v>7.13</v>
       </c>
       <c r="H9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="13">
-        <v>49.933333333333337</v>
+        <v>56.844999999999999</v>
       </c>
       <c r="F10" s="13">
-        <v>10.130000000000001</v>
+        <v>18.295000000000002</v>
       </c>
       <c r="G10" s="13">
-        <v>6.6133333333333342</v>
+        <v>10.004999999999999</v>
       </c>
       <c r="H10" t="s">
         <v>1</v>
@@ -19626,25 +19626,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="13">
-        <v>49.083333333333336</v>
+        <v>59.370000000000005</v>
       </c>
       <c r="F11" s="13">
-        <v>11.913333333333334</v>
+        <v>20.035</v>
       </c>
       <c r="G11" s="13">
-        <v>6.54</v>
+        <v>12.39</v>
       </c>
       <c r="H11" t="s">
         <v>2</v>
@@ -19655,7 +19655,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -19664,16 +19664,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="13">
-        <v>54.879999999999995</v>
+        <v>59.75</v>
       </c>
       <c r="F12" s="13">
-        <v>18.634999999999998</v>
+        <v>15.795</v>
       </c>
       <c r="G12" s="13">
-        <v>9.6449999999999996</v>
+        <v>9.93</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
@@ -19684,7 +19684,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -19693,16 +19693,16 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E13" s="13">
-        <v>54.86</v>
+        <v>54.225000000000001</v>
       </c>
       <c r="F13" s="13">
-        <v>18.66</v>
+        <v>21.34</v>
       </c>
       <c r="G13" s="13">
-        <v>9.27</v>
+        <v>12.395</v>
       </c>
       <c r="H13" t="s">
         <v>2</v>
@@ -19713,141 +19713,141 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="13">
-        <v>43.37</v>
+        <v>55.32</v>
       </c>
       <c r="F14" s="13">
-        <v>20.414999999999999</v>
+        <v>19.36</v>
       </c>
       <c r="G14" s="13">
-        <v>12.565000000000001</v>
+        <v>10.63</v>
       </c>
       <c r="H14" t="s">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E15" s="13">
-        <v>41.11</v>
+        <v>58.49</v>
       </c>
       <c r="F15" s="13">
-        <v>17.299999999999997</v>
+        <v>17.62</v>
       </c>
       <c r="G15" s="13">
-        <v>10.515000000000001</v>
+        <v>9.75</v>
       </c>
       <c r="H15" t="s">
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="13">
-        <v>41.58</v>
+        <v>51.69</v>
       </c>
       <c r="F16" s="13">
-        <v>17.310000000000002</v>
+        <v>20.27</v>
       </c>
       <c r="G16" s="13">
-        <v>12.025</v>
+        <v>10.07</v>
       </c>
       <c r="H16" t="s">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E17" s="13">
-        <v>39.82</v>
+        <v>54.01</v>
       </c>
       <c r="F17" s="13">
-        <v>14.76</v>
+        <v>16.14</v>
       </c>
       <c r="G17" s="13">
-        <v>10.145</v>
+        <v>7.15</v>
       </c>
       <c r="H17" t="s">
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E18" s="13">
-        <v>44.636666666666663</v>
+        <v>52.96</v>
       </c>
       <c r="F18" s="13">
-        <v>7.79</v>
+        <v>12.84</v>
       </c>
       <c r="G18" s="13">
-        <v>9.7966666666666669</v>
+        <v>6.2899999999999991</v>
       </c>
       <c r="H18" t="s">
         <v>1</v>
@@ -19858,25 +19858,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E19" s="13">
-        <v>47.713333333333331</v>
+        <v>60.244999999999997</v>
       </c>
       <c r="F19" s="13">
-        <v>9.56</v>
+        <v>12.615</v>
       </c>
       <c r="G19" s="13">
-        <v>6.8</v>
+        <v>7.7850000000000001</v>
       </c>
       <c r="H19" t="s">
         <v>2</v>
@@ -19887,25 +19887,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20" s="13">
-        <v>49.589999999999996</v>
+        <v>61.034999999999997</v>
       </c>
       <c r="F20" s="13">
-        <v>7.3466666666666667</v>
+        <v>16.004999999999999</v>
       </c>
       <c r="G20" s="13">
-        <v>7.0666666666666664</v>
+        <v>10.254999999999999</v>
       </c>
       <c r="H20" t="s">
         <v>1</v>
@@ -19916,25 +19916,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E21" s="13">
-        <v>49.043333333333329</v>
+        <v>50.32</v>
       </c>
       <c r="F21" s="13">
-        <v>9.1833333333333336</v>
+        <v>15.414999999999999</v>
       </c>
       <c r="G21" s="13">
-        <v>6.7399999999999993</v>
+        <v>7.37</v>
       </c>
       <c r="H21" t="s">
         <v>2</v>
@@ -19945,7 +19945,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -19954,16 +19954,16 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E22" s="13">
-        <v>59.03</v>
+        <v>51.25</v>
       </c>
       <c r="F22" s="13">
-        <v>15.17</v>
+        <v>17.059999999999999</v>
       </c>
       <c r="G22" s="13">
-        <v>8.31</v>
+        <v>7.98</v>
       </c>
       <c r="H22" t="s">
         <v>1</v>
@@ -19974,7 +19974,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -19983,16 +19983,16 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E23" s="13">
-        <v>52.96</v>
+        <v>50.51</v>
       </c>
       <c r="F23" s="13">
-        <v>15.24</v>
+        <v>16.77</v>
       </c>
       <c r="G23" s="13">
-        <v>7.02</v>
+        <v>7.33</v>
       </c>
       <c r="H23" t="s">
         <v>2</v>
@@ -20003,25 +20003,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" s="13">
-        <v>47.91</v>
+        <v>49.27</v>
       </c>
       <c r="F24" s="13">
-        <v>18.37</v>
+        <v>16.96</v>
       </c>
       <c r="G24" s="13">
-        <v>10.120000000000001</v>
+        <v>7.22</v>
       </c>
       <c r="H24" t="s">
         <v>1</v>
@@ -20032,25 +20032,25 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E25" s="13">
-        <v>52.984999999999999</v>
+        <v>51.55</v>
       </c>
       <c r="F25" s="13">
-        <v>19.060000000000002</v>
+        <v>16.47</v>
       </c>
       <c r="G25" s="13">
-        <v>10.25</v>
+        <v>7.37</v>
       </c>
       <c r="H25" t="s">
         <v>2</v>
@@ -20067,25 +20067,25 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="13">
-        <v>45.9</v>
+        <v>48.349999999999994</v>
       </c>
       <c r="F26" s="13">
-        <v>11.555</v>
+        <v>14.625</v>
       </c>
       <c r="G26" s="13">
-        <v>9.495000000000001</v>
+        <v>8.01</v>
       </c>
       <c r="H26" t="s">
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -20096,25 +20096,25 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" s="13">
-        <v>51.134999999999998</v>
+        <v>50.08</v>
       </c>
       <c r="F27" s="13">
-        <v>15.855</v>
+        <v>17.325000000000003</v>
       </c>
       <c r="G27" s="13">
-        <v>9.8550000000000004</v>
+        <v>9.0599999999999987</v>
       </c>
       <c r="H27" t="s">
         <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -20122,28 +20122,28 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" s="13">
-        <v>50.476666666666667</v>
+        <v>43.37</v>
       </c>
       <c r="F28" s="13">
-        <v>6.7433333333333332</v>
+        <v>20.414999999999999</v>
       </c>
       <c r="G28" s="13">
-        <v>7.4433333333333342</v>
+        <v>12.565000000000001</v>
       </c>
       <c r="H28" t="s">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -20151,28 +20151,28 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" s="13">
-        <v>51.456666666666671</v>
+        <v>41.11</v>
       </c>
       <c r="F29" s="13">
-        <v>7.84</v>
+        <v>17.299999999999997</v>
       </c>
       <c r="G29" s="13">
-        <v>6.5166666666666666</v>
+        <v>10.515000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -20183,19 +20183,19 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" s="13">
-        <v>53.31666666666667</v>
+        <v>47.91</v>
       </c>
       <c r="F30" s="13">
-        <v>8.3233333333333324</v>
+        <v>18.37</v>
       </c>
       <c r="G30" s="13">
-        <v>6.7700000000000005</v>
+        <v>10.120000000000001</v>
       </c>
       <c r="H30" t="s">
         <v>1</v>
@@ -20212,19 +20212,19 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" s="13">
-        <v>51.81</v>
+        <v>52.984999999999999</v>
       </c>
       <c r="F31" s="13">
-        <v>7.373333333333334</v>
+        <v>19.060000000000002</v>
       </c>
       <c r="G31" s="13">
-        <v>6.1999999999999993</v>
+        <v>10.25</v>
       </c>
       <c r="H31" t="s">
         <v>2</v>
@@ -20241,19 +20241,19 @@
         <v>5</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" s="13">
-        <v>52.41</v>
+        <v>47.375</v>
       </c>
       <c r="F32" s="13">
-        <v>15.7</v>
+        <v>22.245000000000001</v>
       </c>
       <c r="G32" s="13">
-        <v>7.71</v>
+        <v>13.815</v>
       </c>
       <c r="H32" t="s">
         <v>1</v>
@@ -20270,22 +20270,22 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" s="13">
-        <v>54.08</v>
+        <v>47.784999999999997</v>
       </c>
       <c r="F33" s="13">
-        <v>16.579999999999998</v>
+        <v>19.740000000000002</v>
       </c>
       <c r="G33" s="13">
-        <v>7.13</v>
+        <v>11.925000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
         <v>4</v>
@@ -20293,141 +20293,141 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E34" s="13">
-        <v>47.375</v>
+        <v>55.78</v>
       </c>
       <c r="F34" s="13">
-        <v>22.245000000000001</v>
+        <v>20.035</v>
       </c>
       <c r="G34" s="13">
-        <v>13.815</v>
+        <v>11.545</v>
       </c>
       <c r="H34" t="s">
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E35" s="13">
-        <v>47.784999999999997</v>
+        <v>52.835000000000001</v>
       </c>
       <c r="F35" s="13">
-        <v>19.740000000000002</v>
+        <v>21.75</v>
       </c>
       <c r="G35" s="13">
-        <v>11.925000000000001</v>
+        <v>13.635</v>
       </c>
       <c r="H35" t="s">
         <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="13">
-        <v>46.024999999999999</v>
+        <v>50.15</v>
       </c>
       <c r="F36" s="13">
-        <v>13.904999999999999</v>
+        <v>19.52</v>
       </c>
       <c r="G36" s="13">
-        <v>13.129999999999999</v>
+        <v>14.185</v>
       </c>
       <c r="H36" t="s">
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E37" s="13">
-        <v>46.295000000000002</v>
+        <v>52.575000000000003</v>
       </c>
       <c r="F37" s="13">
-        <v>14.45</v>
+        <v>19.385000000000002</v>
       </c>
       <c r="G37" s="13">
-        <v>11.574999999999999</v>
+        <v>12.2</v>
       </c>
       <c r="H37" t="s">
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C38">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E38" s="13">
-        <v>47.54</v>
+        <v>57.635000000000005</v>
       </c>
       <c r="F38" s="13">
-        <v>8.1366666666666667</v>
+        <v>17.744999999999997</v>
       </c>
       <c r="G38" s="13">
-        <v>7.6433333333333335</v>
+        <v>8.27</v>
       </c>
       <c r="H38" t="s">
         <v>1</v>
@@ -20438,25 +20438,25 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E39" s="13">
-        <v>46.576666666666675</v>
+        <v>60.454999999999998</v>
       </c>
       <c r="F39" s="13">
-        <v>7.2600000000000007</v>
+        <v>17.295000000000002</v>
       </c>
       <c r="G39" s="13">
-        <v>9.0833333333333339</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="H39" t="s">
         <v>2</v>
@@ -20467,25 +20467,25 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
       <c r="C40">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" s="13">
-        <v>48.446666666666665</v>
+        <v>50.06</v>
       </c>
       <c r="F40" s="13">
-        <v>7.7399999999999993</v>
+        <v>22.315000000000001</v>
       </c>
       <c r="G40" s="13">
-        <v>7.583333333333333</v>
+        <v>8.36</v>
       </c>
       <c r="H40" t="s">
         <v>1</v>
@@ -20496,25 +20496,25 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" s="13">
-        <v>50.393333333333338</v>
+        <v>49.49</v>
       </c>
       <c r="F41" s="13">
-        <v>7.956666666666667</v>
+        <v>21.91</v>
       </c>
       <c r="G41" s="13">
-        <v>7.41</v>
+        <v>10.805</v>
       </c>
       <c r="H41" t="s">
         <v>2</v>
@@ -20525,25 +20525,25 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42" s="13">
-        <v>56.844999999999999</v>
+        <v>51.800000000000004</v>
       </c>
       <c r="F42" s="13">
-        <v>18.295000000000002</v>
+        <v>17.41</v>
       </c>
       <c r="G42" s="13">
-        <v>10.004999999999999</v>
+        <v>9.91</v>
       </c>
       <c r="H42" t="s">
         <v>1</v>
@@ -20554,25 +20554,25 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E43" s="13">
-        <v>59.370000000000005</v>
+        <v>52.403333333333336</v>
       </c>
       <c r="F43" s="13">
-        <v>20.035</v>
+        <v>14.686666666666667</v>
       </c>
       <c r="G43" s="13">
-        <v>12.39</v>
+        <v>7.3266666666666653</v>
       </c>
       <c r="H43" t="s">
         <v>2</v>
@@ -20583,25 +20583,25 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>3</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E44" s="13">
-        <v>55.78</v>
+        <v>52.083333333333336</v>
       </c>
       <c r="F44" s="13">
-        <v>20.035</v>
+        <v>12.209999999999999</v>
       </c>
       <c r="G44" s="13">
-        <v>11.545</v>
+        <v>8.4233333333333338</v>
       </c>
       <c r="H44" t="s">
         <v>1</v>
@@ -20612,25 +20612,25 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E45" s="13">
-        <v>52.835000000000001</v>
+        <v>47.276666666666664</v>
       </c>
       <c r="F45" s="13">
-        <v>21.75</v>
+        <v>16.540000000000003</v>
       </c>
       <c r="G45" s="13">
-        <v>13.635</v>
+        <v>9.76</v>
       </c>
       <c r="H45" t="s">
         <v>2</v>
@@ -20641,141 +20641,141 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E46" s="13">
-        <v>56.265000000000001</v>
+        <v>51.389999999999993</v>
       </c>
       <c r="F46" s="13">
-        <v>20.725000000000001</v>
+        <v>17.706666666666667</v>
       </c>
       <c r="G46" s="13">
-        <v>14.844999999999999</v>
+        <v>8.8633333333333333</v>
       </c>
       <c r="H46" t="s">
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47" s="13">
+        <v>51.890000000000008</v>
+      </c>
+      <c r="F47" s="13">
+        <v>15.74</v>
+      </c>
+      <c r="G47" s="13">
+        <v>9.1533333333333342</v>
+      </c>
+      <c r="H47" t="s">
+        <v>2</v>
+      </c>
+      <c r="I47" t="s">
         <v>4</v>
-      </c>
-      <c r="E47" s="13">
-        <v>50.2</v>
-      </c>
-      <c r="F47" s="13">
-        <v>19.079999999999998</v>
-      </c>
-      <c r="G47" s="13">
-        <v>10.655000000000001</v>
-      </c>
-      <c r="H47" t="s">
-        <v>2</v>
-      </c>
-      <c r="I47" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48" s="13">
-        <v>53.506666666666661</v>
+        <v>50.74</v>
       </c>
       <c r="F48" s="13">
-        <v>16.336666666666666</v>
+        <v>14.566666666666668</v>
       </c>
       <c r="G48" s="13">
-        <v>10.006666666666666</v>
+        <v>7.2733333333333334</v>
       </c>
       <c r="H48" t="s">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49" s="13">
+        <v>55.793333333333329</v>
+      </c>
+      <c r="F49" s="13">
+        <v>13.089999999999998</v>
+      </c>
+      <c r="G49" s="13">
+        <v>7.7200000000000015</v>
+      </c>
+      <c r="H49" t="s">
+        <v>2</v>
+      </c>
+      <c r="I49" t="s">
         <v>4</v>
-      </c>
-      <c r="E49" s="13">
-        <v>53.636666666666677</v>
-      </c>
-      <c r="F49" s="13">
-        <v>19.326666666666664</v>
-      </c>
-      <c r="G49" s="13">
-        <v>13.633333333333333</v>
-      </c>
-      <c r="H49" t="s">
-        <v>2</v>
-      </c>
-      <c r="I49" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
       <c r="C50">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" s="13">
-        <v>57.830000000000005</v>
+        <v>46.234999999999999</v>
       </c>
       <c r="F50" s="13">
-        <v>13.3866666666667</v>
+        <v>12.31</v>
       </c>
       <c r="G50" s="13">
-        <v>9.5299999999999994</v>
+        <v>7.665</v>
       </c>
       <c r="H50" t="s">
         <v>1</v>
@@ -20786,25 +20786,25 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
       <c r="C51">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E51" s="13">
-        <v>57.699999999999996</v>
+        <v>48.094999999999999</v>
       </c>
       <c r="F51" s="13">
-        <v>11.49</v>
+        <v>14.91</v>
       </c>
       <c r="G51" s="13">
-        <v>7.8133333333333335</v>
+        <v>8.66</v>
       </c>
       <c r="H51" t="s">
         <v>2</v>
@@ -20815,25 +20815,25 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E52" s="13">
-        <v>59.75</v>
+        <v>41.58</v>
       </c>
       <c r="F52" s="13">
-        <v>15.795</v>
+        <v>17.310000000000002</v>
       </c>
       <c r="G52" s="13">
-        <v>9.93</v>
+        <v>12.025</v>
       </c>
       <c r="H52" t="s">
         <v>1</v>
@@ -20844,25 +20844,25 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E53" s="13">
-        <v>54.225000000000001</v>
+        <v>39.82</v>
       </c>
       <c r="F53" s="13">
-        <v>21.34</v>
+        <v>14.76</v>
       </c>
       <c r="G53" s="13">
-        <v>12.395</v>
+        <v>10.145</v>
       </c>
       <c r="H53" t="s">
         <v>2</v>
@@ -20873,65 +20873,65 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E54" s="13">
-        <v>50.15</v>
+        <v>45.9</v>
       </c>
       <c r="F54" s="13">
-        <v>19.52</v>
+        <v>11.555</v>
       </c>
       <c r="G54" s="13">
-        <v>14.185</v>
+        <v>9.495000000000001</v>
       </c>
       <c r="H54" t="s">
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55" s="13">
+        <v>51.134999999999998</v>
+      </c>
+      <c r="F55" s="13">
+        <v>15.855</v>
+      </c>
+      <c r="G55" s="13">
+        <v>9.8550000000000004</v>
+      </c>
+      <c r="H55" t="s">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
         <v>4</v>
-      </c>
-      <c r="E55" s="13">
-        <v>52.575000000000003</v>
-      </c>
-      <c r="F55" s="13">
-        <v>19.385000000000002</v>
-      </c>
-      <c r="G55" s="13">
-        <v>12.2</v>
-      </c>
-      <c r="H55" t="s">
-        <v>2</v>
-      </c>
-      <c r="I55" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
@@ -20940,27 +20940,27 @@
         <v>6</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E56" s="13">
-        <v>51.42</v>
+        <v>46.024999999999999</v>
       </c>
       <c r="F56" s="13">
-        <v>20.425000000000001</v>
+        <v>13.904999999999999</v>
       </c>
       <c r="G56" s="13">
-        <v>11.405000000000001</v>
+        <v>13.129999999999999</v>
       </c>
       <c r="H56" t="s">
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -20969,22 +20969,22 @@
         <v>6</v>
       </c>
       <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" s="13">
+        <v>46.295000000000002</v>
+      </c>
+      <c r="F57" s="13">
+        <v>14.45</v>
+      </c>
+      <c r="G57" s="13">
+        <v>11.574999999999999</v>
+      </c>
+      <c r="H57" t="s">
+        <v>2</v>
+      </c>
+      <c r="I57" t="s">
         <v>4</v>
-      </c>
-      <c r="E57" s="13">
-        <v>46.984999999999999</v>
-      </c>
-      <c r="F57" s="13">
-        <v>16.39</v>
-      </c>
-      <c r="G57" s="13">
-        <v>11.100000000000001</v>
-      </c>
-      <c r="H57" t="s">
-        <v>2</v>
-      </c>
-      <c r="I57" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -20992,22 +20992,22 @@
         <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D58">
         <v>3</v>
       </c>
       <c r="E58" s="13">
-        <v>48.053333333333335</v>
+        <v>56.265000000000001</v>
       </c>
       <c r="F58" s="13">
-        <v>20.563333333333333</v>
+        <v>20.725000000000001</v>
       </c>
       <c r="G58" s="13">
-        <v>12.800000000000002</v>
+        <v>14.844999999999999</v>
       </c>
       <c r="H58" t="s">
         <v>1</v>
@@ -21021,22 +21021,22 @@
         <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D59">
         <v>4</v>
       </c>
       <c r="E59" s="13">
-        <v>50.356666666666662</v>
+        <v>50.2</v>
       </c>
       <c r="F59" s="13">
-        <v>20.603333333333335</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="G59" s="13">
-        <v>12.62</v>
+        <v>10.655000000000001</v>
       </c>
       <c r="H59" t="s">
         <v>2</v>
@@ -21047,25 +21047,25 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
       </c>
       <c r="C60">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D60">
         <v>3</v>
       </c>
       <c r="E60" s="13">
-        <v>54.81</v>
+        <v>51.42</v>
       </c>
       <c r="F60" s="13">
-        <v>11.893333333333333</v>
+        <v>20.425000000000001</v>
       </c>
       <c r="G60" s="13">
-        <v>8.7433333333333341</v>
+        <v>11.405000000000001</v>
       </c>
       <c r="H60" t="s">
         <v>1</v>
@@ -21076,25 +21076,25 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
       </c>
       <c r="C61">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61" s="13">
-        <v>53.393333333333338</v>
+        <v>46.984999999999999</v>
       </c>
       <c r="F61" s="13">
-        <v>14.356666666666667</v>
+        <v>16.39</v>
       </c>
       <c r="G61" s="13">
-        <v>8.61</v>
+        <v>11.100000000000001</v>
       </c>
       <c r="H61" t="s">
         <v>2</v>
@@ -21111,19 +21111,19 @@
         <v>6</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D62">
         <v>3</v>
       </c>
       <c r="E62" s="13">
-        <v>55.32</v>
+        <v>60.19</v>
       </c>
       <c r="F62" s="13">
-        <v>19.36</v>
+        <v>15.7</v>
       </c>
       <c r="G62" s="13">
-        <v>10.63</v>
+        <v>9.14</v>
       </c>
       <c r="H62" t="s">
         <v>1</v>
@@ -21140,19 +21140,19 @@
         <v>6</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D63">
         <v>4</v>
       </c>
       <c r="E63" s="13">
-        <v>58.49</v>
+        <v>53.17</v>
       </c>
       <c r="F63" s="13">
-        <v>17.62</v>
+        <v>17.534999999999997</v>
       </c>
       <c r="G63" s="13">
-        <v>9.75</v>
+        <v>9.7650000000000006</v>
       </c>
       <c r="H63" t="s">
         <v>2</v>
@@ -21166,22 +21166,22 @@
         <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D64">
         <v>3</v>
       </c>
       <c r="E64" s="13">
-        <v>57.635000000000005</v>
+        <v>48.055</v>
       </c>
       <c r="F64" s="13">
-        <v>17.744999999999997</v>
+        <v>20.195</v>
       </c>
       <c r="G64" s="13">
-        <v>8.27</v>
+        <v>11.725</v>
       </c>
       <c r="H64" t="s">
         <v>1</v>
@@ -21195,22 +21195,22 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D65">
         <v>4</v>
       </c>
       <c r="E65" s="13">
-        <v>60.454999999999998</v>
+        <v>46.72</v>
       </c>
       <c r="F65" s="13">
-        <v>17.295000000000002</v>
+        <v>22.325000000000003</v>
       </c>
       <c r="G65" s="13">
-        <v>8.620000000000001</v>
+        <v>13.219999999999999</v>
       </c>
       <c r="H65" t="s">
         <v>2</v>
@@ -21221,7 +21221,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -21230,27 +21230,27 @@
         <v>6</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E66" s="13">
-        <v>60.19</v>
+        <v>51.763333333333328</v>
       </c>
       <c r="F66" s="13">
-        <v>15.7</v>
+        <v>15.006666666666666</v>
       </c>
       <c r="G66" s="13">
-        <v>9.14</v>
+        <v>7.9766666666666666</v>
       </c>
       <c r="H66" t="s">
         <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
@@ -21259,103 +21259,103 @@
         <v>6</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E67" s="13">
-        <v>53.17</v>
+        <v>49.6</v>
       </c>
       <c r="F67" s="13">
-        <v>17.534999999999997</v>
+        <v>14.723333333333334</v>
       </c>
       <c r="G67" s="13">
-        <v>9.7650000000000006</v>
+        <v>7.2833333333333323</v>
       </c>
       <c r="H67" t="s">
         <v>2</v>
       </c>
       <c r="I67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E68" s="13">
-        <v>51.946666666666665</v>
+        <v>51.376666666666665</v>
       </c>
       <c r="F68" s="13">
-        <v>15.076666666666668</v>
+        <v>13.663333333333334</v>
       </c>
       <c r="G68" s="13">
-        <v>9.3166666666666647</v>
+        <v>5.8366666666666669</v>
       </c>
       <c r="H68" t="s">
         <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D69">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E69" s="13">
-        <v>54.926666666666669</v>
+        <v>46.696666666666658</v>
       </c>
       <c r="F69" s="13">
-        <v>12.660000000000002</v>
+        <v>13.82</v>
       </c>
       <c r="G69" s="13">
-        <v>6.68</v>
+        <v>7.0933333333333337</v>
       </c>
       <c r="H69" t="s">
         <v>2</v>
       </c>
       <c r="I69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
       </c>
       <c r="C70">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E70" s="13">
-        <v>56.006666666666668</v>
+        <v>51.316666666666663</v>
       </c>
       <c r="F70" s="13">
-        <v>11.283333333333333</v>
+        <v>13.443333333333333</v>
       </c>
       <c r="G70" s="13">
-        <v>7.6000000000000005</v>
+        <v>6.73</v>
       </c>
       <c r="H70" t="s">
         <v>1</v>
@@ -21366,25 +21366,25 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
       </c>
       <c r="C71">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E71" s="13">
-        <v>55.78</v>
+        <v>52.946666666666665</v>
       </c>
       <c r="F71" s="13">
-        <v>11.083333333333334</v>
+        <v>13.553333333333335</v>
       </c>
       <c r="G71" s="13">
-        <v>5.6303333333333327</v>
+        <v>7.0233333333333334</v>
       </c>
       <c r="H71" t="s">
         <v>2</v>
@@ -21395,25 +21395,25 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E72" s="13">
-        <v>51.69</v>
+        <v>52.983333333333327</v>
       </c>
       <c r="F72" s="13">
-        <v>20.27</v>
+        <v>8.9466666666666672</v>
       </c>
       <c r="G72" s="13">
-        <v>10.07</v>
+        <v>7.7333333333333334</v>
       </c>
       <c r="H72" t="s">
         <v>1</v>
@@ -21424,25 +21424,25 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D73">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E73" s="13">
-        <v>54.01</v>
+        <v>45.96</v>
       </c>
       <c r="F73" s="13">
-        <v>16.14</v>
+        <v>9.9033333333333342</v>
       </c>
       <c r="G73" s="13">
-        <v>7.15</v>
+        <v>7.836666666666666</v>
       </c>
       <c r="H73" t="s">
         <v>2</v>
@@ -21453,141 +21453,141 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74" s="13">
-        <v>50.06</v>
+        <v>48.85</v>
       </c>
       <c r="F74" s="13">
-        <v>22.315000000000001</v>
+        <v>10.733333333333334</v>
       </c>
       <c r="G74" s="13">
-        <v>8.36</v>
+        <v>8.2266666666666666</v>
       </c>
       <c r="H74" t="s">
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E75" s="13">
-        <v>49.49</v>
+        <v>48</v>
       </c>
       <c r="F75" s="13">
-        <v>21.91</v>
+        <v>12.526666666666666</v>
       </c>
       <c r="G75" s="13">
-        <v>10.805</v>
+        <v>6.7600000000000007</v>
       </c>
       <c r="H75" t="s">
         <v>2</v>
       </c>
       <c r="I75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
       <c r="C76">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E76" s="13">
-        <v>48.055</v>
+        <v>44.636666666666663</v>
       </c>
       <c r="F76" s="13">
-        <v>20.195</v>
+        <v>7.79</v>
       </c>
       <c r="G76" s="13">
-        <v>11.725</v>
+        <v>9.7966666666666669</v>
       </c>
       <c r="H76" t="s">
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
       <c r="C77">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E77" s="13">
-        <v>46.72</v>
+        <v>47.713333333333331</v>
       </c>
       <c r="F77" s="13">
-        <v>22.325000000000003</v>
+        <v>9.56</v>
       </c>
       <c r="G77" s="13">
-        <v>13.219999999999999</v>
+        <v>6.8</v>
       </c>
       <c r="H77" t="s">
         <v>2</v>
       </c>
       <c r="I77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C78">
         <v>9</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E78" s="13">
-        <v>54.5</v>
+        <v>50.476666666666667</v>
       </c>
       <c r="F78" s="13">
-        <v>17.220000000000002</v>
+        <v>6.7433333333333332</v>
       </c>
       <c r="G78" s="13">
-        <v>9.2000000000000011</v>
+        <v>7.4433333333333342</v>
       </c>
       <c r="H78" t="s">
         <v>1</v>
@@ -21598,25 +21598,25 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C79">
         <v>9</v>
       </c>
       <c r="D79">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E79" s="13">
-        <v>46.393333333333338</v>
+        <v>51.456666666666671</v>
       </c>
       <c r="F79" s="13">
-        <v>18.393333333333334</v>
+        <v>7.84</v>
       </c>
       <c r="G79" s="13">
-        <v>10.946666666666665</v>
+        <v>6.5166666666666666</v>
       </c>
       <c r="H79" t="s">
         <v>2</v>
@@ -21627,25 +21627,25 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B80" t="s">
         <v>5</v>
       </c>
       <c r="C80">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E80" s="13">
-        <v>54.036666666666662</v>
+        <v>47.54</v>
       </c>
       <c r="F80" s="13">
-        <v>6.8633333333333333</v>
+        <v>8.1366666666666667</v>
       </c>
       <c r="G80" s="13">
-        <v>6.1966666666666663</v>
+        <v>7.6433333333333335</v>
       </c>
       <c r="H80" t="s">
         <v>1</v>
@@ -21656,25 +21656,25 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="C81">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D81">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E81" s="13">
-        <v>55.94</v>
+        <v>46.576666666666675</v>
       </c>
       <c r="F81" s="13">
-        <v>9.2000000000000011</v>
+        <v>7.2600000000000007</v>
       </c>
       <c r="G81" s="13">
-        <v>6.55</v>
+        <v>9.0833333333333339</v>
       </c>
       <c r="H81" t="s">
         <v>2</v>
@@ -21685,25 +21685,25 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D82">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E82" s="13">
-        <v>52.96</v>
+        <v>53.506666666666661</v>
       </c>
       <c r="F82" s="13">
-        <v>12.84</v>
+        <v>16.336666666666666</v>
       </c>
       <c r="G82" s="13">
-        <v>6.2899999999999991</v>
+        <v>10.006666666666666</v>
       </c>
       <c r="H82" t="s">
         <v>1</v>
@@ -21714,25 +21714,25 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D83">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E83" s="13">
-        <v>60.244999999999997</v>
+        <v>53.636666666666677</v>
       </c>
       <c r="F83" s="13">
-        <v>12.615</v>
+        <v>19.326666666666664</v>
       </c>
       <c r="G83" s="13">
-        <v>7.7850000000000001</v>
+        <v>13.633333333333333</v>
       </c>
       <c r="H83" t="s">
         <v>2</v>
@@ -21743,25 +21743,25 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D84">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E84" s="13">
-        <v>51.800000000000004</v>
+        <v>48.053333333333335</v>
       </c>
       <c r="F84" s="13">
-        <v>17.41</v>
+        <v>20.563333333333333</v>
       </c>
       <c r="G84" s="13">
-        <v>9.91</v>
+        <v>12.800000000000002</v>
       </c>
       <c r="H84" t="s">
         <v>1</v>
@@ -21772,25 +21772,25 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D85">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E85" s="13">
-        <v>52.403333333333336</v>
+        <v>50.356666666666662</v>
       </c>
       <c r="F85" s="13">
-        <v>14.686666666666667</v>
+        <v>20.603333333333335</v>
       </c>
       <c r="G85" s="13">
-        <v>7.3266666666666653</v>
+        <v>12.62</v>
       </c>
       <c r="H85" t="s">
         <v>2</v>
@@ -21801,118 +21801,118 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
       </c>
       <c r="C86">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D86">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E86" s="13">
-        <v>51.763333333333328</v>
+        <v>51.946666666666665</v>
       </c>
       <c r="F86" s="13">
-        <v>15.006666666666666</v>
+        <v>15.076666666666668</v>
       </c>
       <c r="G86" s="13">
-        <v>7.9766666666666666</v>
+        <v>9.3166666666666647</v>
       </c>
       <c r="H86" t="s">
         <v>1</v>
       </c>
       <c r="I86" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
       </c>
       <c r="C87">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D87">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E87" s="13">
-        <v>49.6</v>
+        <v>54.926666666666669</v>
       </c>
       <c r="F87" s="13">
-        <v>14.723333333333334</v>
+        <v>12.660000000000002</v>
       </c>
       <c r="G87" s="13">
-        <v>7.2833333333333323</v>
+        <v>6.68</v>
       </c>
       <c r="H87" t="s">
         <v>2</v>
       </c>
       <c r="I87" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C88">
         <v>9</v>
       </c>
       <c r="D88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E88" s="13">
-        <v>47.53</v>
+        <v>54.5</v>
       </c>
       <c r="F88" s="13">
-        <v>16.223333333333333</v>
+        <v>17.220000000000002</v>
       </c>
       <c r="G88" s="13">
-        <v>9.74</v>
+        <v>9.2000000000000011</v>
       </c>
       <c r="H88" t="s">
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>9</v>
       </c>
       <c r="D89">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E89" s="13">
-        <v>44.363333333333337</v>
+        <v>46.393333333333338</v>
       </c>
       <c r="F89" s="13">
-        <v>17.056666666666668</v>
+        <v>18.393333333333334</v>
       </c>
       <c r="G89" s="13">
-        <v>10.263333333333334</v>
+        <v>10.946666666666665</v>
       </c>
       <c r="H89" t="s">
         <v>2</v>
       </c>
       <c r="I89" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -21923,19 +21923,19 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D90">
         <v>5</v>
       </c>
       <c r="E90" s="13">
-        <v>49.19</v>
+        <v>47.53</v>
       </c>
       <c r="F90" s="13">
-        <v>6.46</v>
+        <v>16.223333333333333</v>
       </c>
       <c r="G90" s="13">
-        <v>7.3466666666666667</v>
+        <v>9.74</v>
       </c>
       <c r="H90" t="s">
         <v>1</v>
@@ -21952,19 +21952,19 @@
         <v>6</v>
       </c>
       <c r="C91">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D91">
         <v>6</v>
       </c>
       <c r="E91" s="13">
-        <v>49.116666666666667</v>
+        <v>44.363333333333337</v>
       </c>
       <c r="F91" s="13">
-        <v>7.1166666666666671</v>
+        <v>17.056666666666668</v>
       </c>
       <c r="G91" s="13">
-        <v>6.7399999999999993</v>
+        <v>10.263333333333334</v>
       </c>
       <c r="H91" t="s">
         <v>2</v>
@@ -21981,19 +21981,19 @@
         <v>5</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D92">
         <v>5</v>
       </c>
       <c r="E92" s="13">
-        <v>61.034999999999997</v>
+        <v>45.766666666666673</v>
       </c>
       <c r="F92" s="13">
-        <v>16.004999999999999</v>
+        <v>15.123333333333335</v>
       </c>
       <c r="G92" s="13">
-        <v>10.254999999999999</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="H92" t="s">
         <v>1</v>
@@ -22010,19 +22010,19 @@
         <v>5</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D93">
         <v>6</v>
       </c>
       <c r="E93" s="13">
-        <v>50.32</v>
+        <v>45.543333333333329</v>
       </c>
       <c r="F93" s="13">
-        <v>15.414999999999999</v>
+        <v>14.62</v>
       </c>
       <c r="G93" s="13">
-        <v>7.37</v>
+        <v>8.7666666666666675</v>
       </c>
       <c r="H93" t="s">
         <v>2</v>
@@ -22036,28 +22036,28 @@
         <v>14</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D94">
         <v>5</v>
       </c>
       <c r="E94" s="13">
-        <v>52.083333333333336</v>
+        <v>49.903333333333336</v>
       </c>
       <c r="F94" s="13">
-        <v>12.209999999999999</v>
+        <v>12.946666666666665</v>
       </c>
       <c r="G94" s="13">
-        <v>8.4233333333333338</v>
+        <v>9.7333333333333325</v>
       </c>
       <c r="H94" t="s">
         <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -22065,28 +22065,28 @@
         <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D95">
         <v>6</v>
       </c>
       <c r="E95" s="13">
-        <v>47.276666666666664</v>
+        <v>49.25</v>
       </c>
       <c r="F95" s="13">
-        <v>16.540000000000003</v>
+        <v>14.86</v>
       </c>
       <c r="G95" s="13">
-        <v>9.76</v>
+        <v>10.069999999999999</v>
       </c>
       <c r="H95" t="s">
         <v>2</v>
       </c>
       <c r="I95" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -22097,25 +22097,25 @@
         <v>5</v>
       </c>
       <c r="C96">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D96">
         <v>5</v>
       </c>
       <c r="E96" s="13">
-        <v>51.376666666666665</v>
+        <v>51.866666666666674</v>
       </c>
       <c r="F96" s="13">
-        <v>13.663333333333334</v>
+        <v>6.4899999999999993</v>
       </c>
       <c r="G96" s="13">
-        <v>5.8366666666666669</v>
+        <v>6.3500000000000005</v>
       </c>
       <c r="H96" t="s">
         <v>1</v>
       </c>
       <c r="I96" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -22126,48 +22126,48 @@
         <v>5</v>
       </c>
       <c r="C97">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D97">
         <v>6</v>
       </c>
       <c r="E97" s="13">
-        <v>46.696666666666658</v>
+        <v>50.73</v>
       </c>
       <c r="F97" s="13">
-        <v>13.82</v>
+        <v>6.086666666666666</v>
       </c>
       <c r="G97" s="13">
-        <v>7.0933333333333337</v>
+        <v>8.4366666666666656</v>
       </c>
       <c r="H97" t="s">
         <v>2</v>
       </c>
       <c r="I97" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C98">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D98">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E98" s="13">
-        <v>45.766666666666673</v>
+        <v>49.933333333333337</v>
       </c>
       <c r="F98" s="13">
-        <v>15.123333333333335</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="G98" s="13">
-        <v>7.1499999999999995</v>
+        <v>6.6133333333333342</v>
       </c>
       <c r="H98" t="s">
         <v>1</v>
@@ -22178,25 +22178,25 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C99">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D99">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E99" s="13">
-        <v>45.543333333333329</v>
+        <v>49.083333333333336</v>
       </c>
       <c r="F99" s="13">
-        <v>14.62</v>
+        <v>11.913333333333334</v>
       </c>
       <c r="G99" s="13">
-        <v>8.7666666666666675</v>
+        <v>6.54</v>
       </c>
       <c r="H99" t="s">
         <v>2</v>
@@ -22207,7 +22207,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
@@ -22216,16 +22216,16 @@
         <v>12</v>
       </c>
       <c r="D100">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E100" s="13">
-        <v>47.633333333333333</v>
+        <v>49.589999999999996</v>
       </c>
       <c r="F100" s="13">
-        <v>9.5899999999999981</v>
+        <v>7.3466666666666667</v>
       </c>
       <c r="G100" s="13">
-        <v>7.1933333333333325</v>
+        <v>7.0666666666666664</v>
       </c>
       <c r="H100" t="s">
         <v>1</v>
@@ -22236,7 +22236,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
@@ -22245,16 +22245,16 @@
         <v>12</v>
       </c>
       <c r="D101">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E101" s="13">
-        <v>48.756666666666668</v>
+        <v>49.043333333333329</v>
       </c>
       <c r="F101" s="13">
-        <v>7.5</v>
+        <v>9.1833333333333336</v>
       </c>
       <c r="G101" s="13">
-        <v>7.1033333333333326</v>
+        <v>6.7399999999999993</v>
       </c>
       <c r="H101" t="s">
         <v>2</v>
@@ -22265,25 +22265,25 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D102">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E102" s="13">
-        <v>51.25</v>
+        <v>53.31666666666667</v>
       </c>
       <c r="F102" s="13">
-        <v>17.059999999999999</v>
+        <v>8.3233333333333324</v>
       </c>
       <c r="G102" s="13">
-        <v>7.98</v>
+        <v>6.7700000000000005</v>
       </c>
       <c r="H102" t="s">
         <v>1</v>
@@ -22294,25 +22294,25 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D103">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E103" s="13">
-        <v>50.51</v>
+        <v>51.81</v>
       </c>
       <c r="F103" s="13">
-        <v>16.77</v>
+        <v>7.373333333333334</v>
       </c>
       <c r="G103" s="13">
-        <v>7.33</v>
+        <v>6.1999999999999993</v>
       </c>
       <c r="H103" t="s">
         <v>2</v>
@@ -22323,25 +22323,25 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D104">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E104" s="13">
-        <v>51.389999999999993</v>
+        <v>48.446666666666665</v>
       </c>
       <c r="F104" s="13">
-        <v>17.706666666666667</v>
+        <v>7.7399999999999993</v>
       </c>
       <c r="G104" s="13">
-        <v>8.8633333333333333</v>
+        <v>7.583333333333333</v>
       </c>
       <c r="H104" t="s">
         <v>1</v>
@@ -22352,25 +22352,25 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D105">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E105" s="13">
-        <v>51.890000000000008</v>
+        <v>50.393333333333338</v>
       </c>
       <c r="F105" s="13">
-        <v>15.74</v>
+        <v>7.956666666666667</v>
       </c>
       <c r="G105" s="13">
-        <v>9.1533333333333342</v>
+        <v>7.41</v>
       </c>
       <c r="H105" t="s">
         <v>2</v>
@@ -22381,123 +22381,123 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
       </c>
       <c r="C106">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D106">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E106" s="13">
-        <v>51.316666666666663</v>
+        <v>57.830000000000005</v>
       </c>
       <c r="F106" s="13">
-        <v>13.443333333333333</v>
+        <v>13.3866666666667</v>
       </c>
       <c r="G106" s="13">
-        <v>6.73</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="H106" t="s">
         <v>1</v>
       </c>
       <c r="I106" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
       </c>
       <c r="C107">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D107">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E107" s="13">
-        <v>52.946666666666665</v>
+        <v>57.699999999999996</v>
       </c>
       <c r="F107" s="13">
-        <v>13.553333333333335</v>
+        <v>11.49</v>
       </c>
       <c r="G107" s="13">
-        <v>7.0233333333333334</v>
+        <v>7.8133333333333335</v>
       </c>
       <c r="H107" t="s">
         <v>2</v>
       </c>
       <c r="I107" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D108">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E108" s="13">
-        <v>49.903333333333336</v>
+        <v>54.81</v>
       </c>
       <c r="F108" s="13">
-        <v>12.946666666666665</v>
+        <v>11.893333333333333</v>
       </c>
       <c r="G108" s="13">
-        <v>9.7333333333333325</v>
+        <v>8.7433333333333341</v>
       </c>
       <c r="H108" t="s">
         <v>1</v>
       </c>
       <c r="I108" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C109">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D109">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E109" s="13">
-        <v>49.25</v>
+        <v>53.393333333333338</v>
       </c>
       <c r="F109" s="13">
-        <v>14.86</v>
+        <v>14.356666666666667</v>
       </c>
       <c r="G109" s="13">
-        <v>10.069999999999999</v>
+        <v>8.61</v>
       </c>
       <c r="H109" t="s">
         <v>2</v>
       </c>
       <c r="I109" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
@@ -22506,16 +22506,16 @@
         <v>12</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E110" s="13">
-        <v>48.233333333333327</v>
+        <v>56.006666666666668</v>
       </c>
       <c r="F110" s="13">
-        <v>6.4933333333333332</v>
+        <v>11.283333333333333</v>
       </c>
       <c r="G110" s="13">
-        <v>7.38</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="H110" t="s">
         <v>1</v>
@@ -22526,7 +22526,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -22535,16 +22535,16 @@
         <v>12</v>
       </c>
       <c r="D111">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E111" s="13">
-        <v>51.859999999999992</v>
+        <v>55.78</v>
       </c>
       <c r="F111" s="13">
-        <v>6.080000000000001</v>
+        <v>11.083333333333334</v>
       </c>
       <c r="G111" s="13">
-        <v>6.7033333333333331</v>
+        <v>5.6303333333333327</v>
       </c>
       <c r="H111" t="s">
         <v>2</v>
@@ -22555,25 +22555,25 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B112" t="s">
         <v>5</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D112">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E112" s="13">
-        <v>49.27</v>
+        <v>54.036666666666662</v>
       </c>
       <c r="F112" s="13">
-        <v>16.96</v>
+        <v>6.8633333333333333</v>
       </c>
       <c r="G112" s="13">
-        <v>7.22</v>
+        <v>6.1966666666666663</v>
       </c>
       <c r="H112" t="s">
         <v>1</v>
@@ -22584,25 +22584,25 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B113" t="s">
         <v>5</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D113">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E113" s="13">
-        <v>51.55</v>
+        <v>55.94</v>
       </c>
       <c r="F113" s="13">
-        <v>16.47</v>
+        <v>9.2000000000000011</v>
       </c>
       <c r="G113" s="13">
-        <v>7.37</v>
+        <v>6.55</v>
       </c>
       <c r="H113" t="s">
         <v>2</v>
@@ -22616,28 +22616,28 @@
         <v>14</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D114">
         <v>5</v>
       </c>
       <c r="E114" s="13">
-        <v>50.74</v>
+        <v>49.19</v>
       </c>
       <c r="F114" s="13">
-        <v>14.566666666666668</v>
+        <v>6.46</v>
       </c>
       <c r="G114" s="13">
-        <v>7.2733333333333334</v>
+        <v>7.3466666666666667</v>
       </c>
       <c r="H114" t="s">
         <v>1</v>
       </c>
       <c r="I114" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -22645,28 +22645,28 @@
         <v>14</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D115">
         <v>6</v>
       </c>
       <c r="E115" s="13">
-        <v>55.793333333333329</v>
+        <v>49.116666666666667</v>
       </c>
       <c r="F115" s="13">
-        <v>13.089999999999998</v>
+        <v>7.1166666666666671</v>
       </c>
       <c r="G115" s="13">
-        <v>7.7200000000000015</v>
+        <v>6.7399999999999993</v>
       </c>
       <c r="H115" t="s">
         <v>2</v>
       </c>
       <c r="I115" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -22677,25 +22677,25 @@
         <v>5</v>
       </c>
       <c r="C116">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D116">
         <v>5</v>
       </c>
       <c r="E116" s="13">
-        <v>52.983333333333327</v>
+        <v>47.633333333333333</v>
       </c>
       <c r="F116" s="13">
-        <v>8.9466666666666672</v>
+        <v>9.5899999999999981</v>
       </c>
       <c r="G116" s="13">
-        <v>7.7333333333333334</v>
+        <v>7.1933333333333325</v>
       </c>
       <c r="H116" t="s">
         <v>1</v>
       </c>
       <c r="I116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -22706,25 +22706,25 @@
         <v>5</v>
       </c>
       <c r="C117">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D117">
         <v>6</v>
       </c>
       <c r="E117" s="13">
-        <v>45.96</v>
+        <v>48.756666666666668</v>
       </c>
       <c r="F117" s="13">
-        <v>9.9033333333333342</v>
+        <v>7.5</v>
       </c>
       <c r="G117" s="13">
-        <v>7.836666666666666</v>
+        <v>7.1033333333333326</v>
       </c>
       <c r="H117" t="s">
         <v>2</v>
       </c>
       <c r="I117" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -22732,22 +22732,22 @@
         <v>14</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D118">
         <v>5</v>
       </c>
       <c r="E118" s="13">
-        <v>51.866666666666674</v>
+        <v>48.233333333333327</v>
       </c>
       <c r="F118" s="13">
-        <v>6.4899999999999993</v>
+        <v>6.4933333333333332</v>
       </c>
       <c r="G118" s="13">
-        <v>6.3500000000000005</v>
+        <v>7.38</v>
       </c>
       <c r="H118" t="s">
         <v>1</v>
@@ -22761,22 +22761,22 @@
         <v>14</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C119">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D119">
         <v>6</v>
       </c>
       <c r="E119" s="13">
-        <v>50.73</v>
+        <v>51.859999999999992</v>
       </c>
       <c r="F119" s="13">
-        <v>6.086666666666666</v>
+        <v>6.080000000000001</v>
       </c>
       <c r="G119" s="13">
-        <v>8.4366666666666656</v>
+        <v>6.7033333333333331</v>
       </c>
       <c r="H119" t="s">
         <v>2</v>
@@ -22846,7 +22846,7 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{BE737EBC-9F60-4B9C-A129-2AF937BFD6AB}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I121">
-      <sortCondition ref="A1"/>
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>